<commit_message>
Neue Version Stand Ende Mai
</commit_message>
<xml_diff>
--- a/Deaths/Germany Cases.xlsx
+++ b/Deaths/Germany Cases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johan\Google Drive\Backup\LwC\Users\JohannAbr\Documents\Corona\Daten\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johan\Google Drive\Backup\LwC\Users\JohannAbr\Documents\Corona\Daten\Deaths\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B441D841-BDE4-43BF-8CCD-00EF76743ACE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CA76D16-1B80-4E77-8B04-47F5F5663FBB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{66B2E3FF-562F-4D86-A698-E4152D9A5061}"/>
   </bookViews>
@@ -437,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECA5C306-C673-43C4-A066-7826087AE258}">
-  <dimension ref="A1:Q56"/>
+  <dimension ref="A1:Q71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="B1:Q1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3413,7 +3413,803 @@
         <v>93</v>
       </c>
     </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A57" s="1">
+        <v>43954</v>
+      </c>
+      <c r="B57">
+        <v>1412</v>
+      </c>
+      <c r="C57">
+        <v>1910</v>
+      </c>
+      <c r="D57">
+        <v>154</v>
+      </c>
+      <c r="E57">
+        <v>122</v>
+      </c>
+      <c r="F57">
+        <v>30</v>
+      </c>
+      <c r="G57">
+        <v>164</v>
+      </c>
+      <c r="H57">
+        <v>370</v>
+      </c>
+      <c r="I57">
+        <v>18</v>
+      </c>
+      <c r="J57">
+        <v>453</v>
+      </c>
+      <c r="K57">
+        <v>1287</v>
+      </c>
+      <c r="L57">
+        <v>176</v>
+      </c>
+      <c r="M57">
+        <v>138</v>
+      </c>
+      <c r="N57">
+        <v>165</v>
+      </c>
+      <c r="O57">
+        <v>44</v>
+      </c>
+      <c r="P57">
+        <v>113</v>
+      </c>
+      <c r="Q57">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A58" s="1">
+        <v>43955</v>
+      </c>
+      <c r="B58">
+        <v>1421</v>
+      </c>
+      <c r="C58">
+        <v>1926</v>
+      </c>
+      <c r="D58">
+        <v>154</v>
+      </c>
+      <c r="E58">
+        <v>122</v>
+      </c>
+      <c r="F58">
+        <v>30</v>
+      </c>
+      <c r="G58">
+        <v>166</v>
+      </c>
+      <c r="H58">
+        <v>372</v>
+      </c>
+      <c r="I58">
+        <v>18</v>
+      </c>
+      <c r="J58">
+        <v>456</v>
+      </c>
+      <c r="K58">
+        <v>1290</v>
+      </c>
+      <c r="L58">
+        <v>177</v>
+      </c>
+      <c r="M58">
+        <v>139</v>
+      </c>
+      <c r="N58">
+        <v>167</v>
+      </c>
+      <c r="O58">
+        <v>45</v>
+      </c>
+      <c r="P58">
+        <v>113</v>
+      </c>
+      <c r="Q58">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A59" s="1">
+        <v>43956</v>
+      </c>
+      <c r="B59">
+        <v>1452</v>
+      </c>
+      <c r="C59">
+        <v>1949</v>
+      </c>
+      <c r="D59">
+        <v>154</v>
+      </c>
+      <c r="E59">
+        <v>123</v>
+      </c>
+      <c r="F59">
+        <v>31</v>
+      </c>
+      <c r="G59">
+        <v>172</v>
+      </c>
+      <c r="H59">
+        <v>381</v>
+      </c>
+      <c r="I59">
+        <v>19</v>
+      </c>
+      <c r="J59">
+        <v>463</v>
+      </c>
+      <c r="K59">
+        <v>1332</v>
+      </c>
+      <c r="L59">
+        <v>182</v>
+      </c>
+      <c r="M59">
+        <v>139</v>
+      </c>
+      <c r="N59">
+        <v>171</v>
+      </c>
+      <c r="O59">
+        <v>46</v>
+      </c>
+      <c r="P59">
+        <v>118</v>
+      </c>
+      <c r="Q59">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A60" s="1">
+        <v>43957</v>
+      </c>
+      <c r="B60">
+        <v>1481</v>
+      </c>
+      <c r="C60">
+        <v>2001</v>
+      </c>
+      <c r="D60">
+        <v>159</v>
+      </c>
+      <c r="E60">
+        <v>127</v>
+      </c>
+      <c r="F60">
+        <v>31</v>
+      </c>
+      <c r="G60">
+        <v>190</v>
+      </c>
+      <c r="H60">
+        <v>386</v>
+      </c>
+      <c r="I60">
+        <v>19</v>
+      </c>
+      <c r="J60">
+        <v>470</v>
+      </c>
+      <c r="K60">
+        <v>1358</v>
+      </c>
+      <c r="L60">
+        <v>187</v>
+      </c>
+      <c r="M60">
+        <v>140</v>
+      </c>
+      <c r="N60">
+        <v>177</v>
+      </c>
+      <c r="O60">
+        <v>46</v>
+      </c>
+      <c r="P60">
+        <v>119</v>
+      </c>
+      <c r="Q60">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A61" s="1">
+        <v>43958</v>
+      </c>
+      <c r="B61">
+        <v>1497</v>
+      </c>
+      <c r="C61">
+        <v>2050</v>
+      </c>
+      <c r="D61">
+        <v>162</v>
+      </c>
+      <c r="E61">
+        <v>129</v>
+      </c>
+      <c r="F61">
+        <v>32</v>
+      </c>
+      <c r="G61">
+        <v>194</v>
+      </c>
+      <c r="H61">
+        <v>396</v>
+      </c>
+      <c r="I61">
+        <v>19</v>
+      </c>
+      <c r="J61">
+        <v>478</v>
+      </c>
+      <c r="K61">
+        <v>1372</v>
+      </c>
+      <c r="L61">
+        <v>189</v>
+      </c>
+      <c r="M61">
+        <v>140</v>
+      </c>
+      <c r="N61">
+        <v>181</v>
+      </c>
+      <c r="O61">
+        <v>48</v>
+      </c>
+      <c r="P61">
+        <v>120</v>
+      </c>
+      <c r="Q61">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A62" s="1">
+        <v>43959</v>
+      </c>
+      <c r="B62">
+        <v>1515</v>
+      </c>
+      <c r="C62">
+        <v>2114</v>
+      </c>
+      <c r="D62">
+        <v>163</v>
+      </c>
+      <c r="E62">
+        <v>131</v>
+      </c>
+      <c r="F62">
+        <v>32</v>
+      </c>
+      <c r="G62">
+        <v>201</v>
+      </c>
+      <c r="H62">
+        <v>403</v>
+      </c>
+      <c r="I62">
+        <v>19</v>
+      </c>
+      <c r="J62">
+        <v>493</v>
+      </c>
+      <c r="K62">
+        <v>1397</v>
+      </c>
+      <c r="L62">
+        <v>192</v>
+      </c>
+      <c r="M62">
+        <v>140</v>
+      </c>
+      <c r="N62">
+        <v>184</v>
+      </c>
+      <c r="O62">
+        <v>48</v>
+      </c>
+      <c r="P62">
+        <v>122</v>
+      </c>
+      <c r="Q62">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A63" s="1">
+        <v>43960</v>
+      </c>
+      <c r="B63">
+        <v>1534</v>
+      </c>
+      <c r="C63">
+        <v>2147</v>
+      </c>
+      <c r="D63">
+        <v>164</v>
+      </c>
+      <c r="E63">
+        <v>133</v>
+      </c>
+      <c r="F63">
+        <v>32</v>
+      </c>
+      <c r="G63">
+        <v>204</v>
+      </c>
+      <c r="H63">
+        <v>408</v>
+      </c>
+      <c r="I63">
+        <v>19</v>
+      </c>
+      <c r="J63">
+        <v>496</v>
+      </c>
+      <c r="K63">
+        <v>1424</v>
+      </c>
+      <c r="L63">
+        <v>195</v>
+      </c>
+      <c r="M63">
+        <v>142</v>
+      </c>
+      <c r="N63">
+        <v>186</v>
+      </c>
+      <c r="O63">
+        <v>48</v>
+      </c>
+      <c r="P63">
+        <v>122</v>
+      </c>
+      <c r="Q63">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A64" s="1">
+        <v>43961</v>
+      </c>
+      <c r="B64">
+        <v>1542</v>
+      </c>
+      <c r="C64">
+        <v>2153</v>
+      </c>
+      <c r="D64">
+        <v>165</v>
+      </c>
+      <c r="E64">
+        <v>134</v>
+      </c>
+      <c r="F64">
+        <v>32</v>
+      </c>
+      <c r="G64">
+        <v>204</v>
+      </c>
+      <c r="H64">
+        <v>411</v>
+      </c>
+      <c r="I64">
+        <v>19</v>
+      </c>
+      <c r="J64">
+        <v>498</v>
+      </c>
+      <c r="K64">
+        <v>1425</v>
+      </c>
+      <c r="L64">
+        <v>195</v>
+      </c>
+      <c r="M64">
+        <v>142</v>
+      </c>
+      <c r="N64">
+        <v>187</v>
+      </c>
+      <c r="O64">
+        <v>48</v>
+      </c>
+      <c r="P64">
+        <v>123</v>
+      </c>
+      <c r="Q64">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A65" s="1">
+        <v>43962</v>
+      </c>
+      <c r="B65">
+        <v>1545</v>
+      </c>
+      <c r="C65">
+        <v>2155</v>
+      </c>
+      <c r="D65">
+        <v>165</v>
+      </c>
+      <c r="E65">
+        <v>134</v>
+      </c>
+      <c r="F65">
+        <v>34</v>
+      </c>
+      <c r="G65">
+        <v>204</v>
+      </c>
+      <c r="H65">
+        <v>412</v>
+      </c>
+      <c r="I65">
+        <v>19</v>
+      </c>
+      <c r="J65">
+        <v>498</v>
+      </c>
+      <c r="K65">
+        <v>1437</v>
+      </c>
+      <c r="L65">
+        <v>195</v>
+      </c>
+      <c r="M65">
+        <v>142</v>
+      </c>
+      <c r="N65">
+        <v>187</v>
+      </c>
+      <c r="O65">
+        <v>48</v>
+      </c>
+      <c r="P65">
+        <v>124</v>
+      </c>
+      <c r="Q65">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A66" s="1">
+        <v>43963</v>
+      </c>
+      <c r="B66">
+        <v>1568</v>
+      </c>
+      <c r="C66">
+        <v>2182</v>
+      </c>
+      <c r="D66">
+        <v>165</v>
+      </c>
+      <c r="E66">
+        <v>136</v>
+      </c>
+      <c r="F66">
+        <v>35</v>
+      </c>
+      <c r="G66">
+        <v>216</v>
+      </c>
+      <c r="H66">
+        <v>415</v>
+      </c>
+      <c r="I66">
+        <v>20</v>
+      </c>
+      <c r="J66">
+        <v>507</v>
+      </c>
+      <c r="K66">
+        <v>1456</v>
+      </c>
+      <c r="L66">
+        <v>206</v>
+      </c>
+      <c r="M66">
+        <v>144</v>
+      </c>
+      <c r="N66">
+        <v>190</v>
+      </c>
+      <c r="O66">
+        <v>50</v>
+      </c>
+      <c r="P66">
+        <v>125</v>
+      </c>
+      <c r="Q66">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A67" s="1">
+        <v>43964</v>
+      </c>
+      <c r="B67">
+        <v>1594</v>
+      </c>
+      <c r="C67">
+        <v>2209</v>
+      </c>
+      <c r="D67">
+        <v>170</v>
+      </c>
+      <c r="E67">
+        <v>137</v>
+      </c>
+      <c r="F67">
+        <v>36</v>
+      </c>
+      <c r="G67">
+        <v>223</v>
+      </c>
+      <c r="H67">
+        <v>419</v>
+      </c>
+      <c r="I67">
+        <v>20</v>
+      </c>
+      <c r="J67">
+        <v>508</v>
+      </c>
+      <c r="K67">
+        <v>1473</v>
+      </c>
+      <c r="L67">
+        <v>207</v>
+      </c>
+      <c r="M67">
+        <v>144</v>
+      </c>
+      <c r="N67">
+        <v>191</v>
+      </c>
+      <c r="O67">
+        <v>52</v>
+      </c>
+      <c r="P67">
+        <v>125</v>
+      </c>
+      <c r="Q67">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A68" s="1">
+        <v>43965</v>
+      </c>
+      <c r="B68">
+        <v>1608</v>
+      </c>
+      <c r="C68">
+        <v>2229</v>
+      </c>
+      <c r="D68">
+        <v>173</v>
+      </c>
+      <c r="E68">
+        <v>138</v>
+      </c>
+      <c r="F68">
+        <v>37</v>
+      </c>
+      <c r="G68">
+        <v>228</v>
+      </c>
+      <c r="H68">
+        <v>423</v>
+      </c>
+      <c r="I68">
+        <v>20</v>
+      </c>
+      <c r="J68">
+        <v>524</v>
+      </c>
+      <c r="K68">
+        <v>1483</v>
+      </c>
+      <c r="L68">
+        <v>212</v>
+      </c>
+      <c r="M68">
+        <v>145</v>
+      </c>
+      <c r="N68">
+        <v>195</v>
+      </c>
+      <c r="O68">
+        <v>52</v>
+      </c>
+      <c r="P68">
+        <v>125</v>
+      </c>
+      <c r="Q68">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A69" s="1">
+        <v>43966</v>
+      </c>
+      <c r="B69">
+        <v>1628</v>
+      </c>
+      <c r="C69">
+        <v>2260</v>
+      </c>
+      <c r="D69">
+        <v>177</v>
+      </c>
+      <c r="E69">
+        <v>148</v>
+      </c>
+      <c r="F69">
+        <v>37</v>
+      </c>
+      <c r="G69">
+        <v>228</v>
+      </c>
+      <c r="H69">
+        <v>429</v>
+      </c>
+      <c r="I69">
+        <v>20</v>
+      </c>
+      <c r="J69">
+        <v>534</v>
+      </c>
+      <c r="K69">
+        <v>1493</v>
+      </c>
+      <c r="L69">
+        <v>213</v>
+      </c>
+      <c r="M69">
+        <v>147</v>
+      </c>
+      <c r="N69">
+        <v>195</v>
+      </c>
+      <c r="O69">
+        <v>54</v>
+      </c>
+      <c r="P69">
+        <v>126</v>
+      </c>
+      <c r="Q69">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A70" s="1">
+        <v>43967</v>
+      </c>
+      <c r="B70">
+        <v>1644</v>
+      </c>
+      <c r="C70">
+        <v>2273</v>
+      </c>
+      <c r="D70">
+        <v>181</v>
+      </c>
+      <c r="E70">
+        <v>149</v>
+      </c>
+      <c r="F70">
+        <v>37</v>
+      </c>
+      <c r="G70">
+        <v>231</v>
+      </c>
+      <c r="H70">
+        <v>432</v>
+      </c>
+      <c r="I70">
+        <v>20</v>
+      </c>
+      <c r="J70">
+        <v>535</v>
+      </c>
+      <c r="K70">
+        <v>1500</v>
+      </c>
+      <c r="L70">
+        <v>216</v>
+      </c>
+      <c r="M70">
+        <v>149</v>
+      </c>
+      <c r="N70">
+        <v>197</v>
+      </c>
+      <c r="O70">
+        <v>54</v>
+      </c>
+      <c r="P70">
+        <v>126</v>
+      </c>
+      <c r="Q70">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A71" s="1">
+        <v>43968</v>
+      </c>
+      <c r="B71">
+        <v>1648</v>
+      </c>
+      <c r="C71">
+        <v>2283</v>
+      </c>
+      <c r="D71">
+        <v>182</v>
+      </c>
+      <c r="E71">
+        <v>149</v>
+      </c>
+      <c r="F71">
+        <v>37</v>
+      </c>
+      <c r="G71">
+        <v>232</v>
+      </c>
+      <c r="H71">
+        <v>435</v>
+      </c>
+      <c r="I71">
+        <v>20</v>
+      </c>
+      <c r="J71">
+        <v>544</v>
+      </c>
+      <c r="K71">
+        <v>1505</v>
+      </c>
+      <c r="L71">
+        <v>216</v>
+      </c>
+      <c r="M71">
+        <v>149</v>
+      </c>
+      <c r="N71">
+        <v>196</v>
+      </c>
+      <c r="O71">
+        <v>54</v>
+      </c>
+      <c r="P71">
+        <v>126</v>
+      </c>
+      <c r="Q71">
+        <v>138</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Dash App integriert und Benni ist Dumm
</commit_message>
<xml_diff>
--- a/Deaths/Germany Cases.xlsx
+++ b/Deaths/Germany Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johan\Google Drive\Backup\LwC\Users\JohannAbr\Documents\Corona\Daten\Deaths\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CA76D16-1B80-4E77-8B04-47F5F5663FBB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B8872D-59F9-490E-8D3F-B84A11D9006C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{66B2E3FF-562F-4D86-A698-E4152D9A5061}"/>
   </bookViews>
@@ -437,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECA5C306-C673-43C4-A066-7826087AE258}">
-  <dimension ref="A1:Q71"/>
+  <dimension ref="A1:Q88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="B89" sqref="B89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4208,6 +4208,907 @@
         <v>138</v>
       </c>
     </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A72" s="1">
+        <v>43969</v>
+      </c>
+      <c r="B72">
+        <v>1652</v>
+      </c>
+      <c r="C72">
+        <v>2287</v>
+      </c>
+      <c r="D72">
+        <v>180</v>
+      </c>
+      <c r="E72">
+        <v>149</v>
+      </c>
+      <c r="F72">
+        <v>38</v>
+      </c>
+      <c r="G72">
+        <v>232</v>
+      </c>
+      <c r="H72">
+        <v>439</v>
+      </c>
+      <c r="I72">
+        <v>20</v>
+      </c>
+      <c r="J72">
+        <v>545</v>
+      </c>
+      <c r="K72">
+        <v>1512</v>
+      </c>
+      <c r="L72">
+        <v>217</v>
+      </c>
+      <c r="M72">
+        <v>149</v>
+      </c>
+      <c r="N72">
+        <v>196</v>
+      </c>
+      <c r="O72">
+        <v>54</v>
+      </c>
+      <c r="P72">
+        <v>126</v>
+      </c>
+      <c r="Q72">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A73" s="1">
+        <v>43970</v>
+      </c>
+      <c r="B73">
+        <v>1653</v>
+      </c>
+      <c r="C73">
+        <v>2314</v>
+      </c>
+      <c r="D73">
+        <v>182</v>
+      </c>
+      <c r="E73">
+        <v>150</v>
+      </c>
+      <c r="F73">
+        <v>38</v>
+      </c>
+      <c r="G73">
+        <v>232</v>
+      </c>
+      <c r="H73">
+        <v>442</v>
+      </c>
+      <c r="I73">
+        <v>20</v>
+      </c>
+      <c r="J73">
+        <v>548</v>
+      </c>
+      <c r="K73">
+        <v>1525</v>
+      </c>
+      <c r="L73">
+        <v>222</v>
+      </c>
+      <c r="M73">
+        <v>154</v>
+      </c>
+      <c r="N73">
+        <v>198</v>
+      </c>
+      <c r="O73">
+        <v>54</v>
+      </c>
+      <c r="P73">
+        <v>128</v>
+      </c>
+      <c r="Q73">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A74" s="1">
+        <v>43971</v>
+      </c>
+      <c r="B74">
+        <v>1672</v>
+      </c>
+      <c r="C74">
+        <v>2339</v>
+      </c>
+      <c r="D74">
+        <v>186</v>
+      </c>
+      <c r="E74">
+        <v>151</v>
+      </c>
+      <c r="F74">
+        <v>38</v>
+      </c>
+      <c r="G74">
+        <v>236</v>
+      </c>
+      <c r="H74">
+        <v>446</v>
+      </c>
+      <c r="I74">
+        <v>20</v>
+      </c>
+      <c r="J74">
+        <v>557</v>
+      </c>
+      <c r="K74">
+        <v>1537</v>
+      </c>
+      <c r="L74">
+        <v>222</v>
+      </c>
+      <c r="M74">
+        <v>154</v>
+      </c>
+      <c r="N74">
+        <v>198</v>
+      </c>
+      <c r="O74">
+        <v>54</v>
+      </c>
+      <c r="P74">
+        <v>131</v>
+      </c>
+      <c r="Q74">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A75" s="1">
+        <v>43972</v>
+      </c>
+      <c r="B75">
+        <v>1680</v>
+      </c>
+      <c r="C75">
+        <v>2348</v>
+      </c>
+      <c r="D75">
+        <v>186</v>
+      </c>
+      <c r="E75">
+        <v>151</v>
+      </c>
+      <c r="F75">
+        <v>39</v>
+      </c>
+      <c r="G75">
+        <v>239</v>
+      </c>
+      <c r="H75">
+        <v>451</v>
+      </c>
+      <c r="I75">
+        <v>20</v>
+      </c>
+      <c r="J75">
+        <v>566</v>
+      </c>
+      <c r="K75">
+        <v>1546</v>
+      </c>
+      <c r="L75">
+        <v>224</v>
+      </c>
+      <c r="M75">
+        <v>157</v>
+      </c>
+      <c r="N75">
+        <v>201</v>
+      </c>
+      <c r="O75">
+        <v>54</v>
+      </c>
+      <c r="P75">
+        <v>134</v>
+      </c>
+      <c r="Q75">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A76" s="1">
+        <v>43973</v>
+      </c>
+      <c r="B76">
+        <v>1680</v>
+      </c>
+      <c r="C76">
+        <v>2358</v>
+      </c>
+      <c r="D76">
+        <v>190</v>
+      </c>
+      <c r="E76">
+        <v>152</v>
+      </c>
+      <c r="F76">
+        <v>39</v>
+      </c>
+      <c r="G76">
+        <v>240</v>
+      </c>
+      <c r="H76">
+        <v>457</v>
+      </c>
+      <c r="I76">
+        <v>20</v>
+      </c>
+      <c r="J76">
+        <v>568</v>
+      </c>
+      <c r="K76">
+        <v>1547</v>
+      </c>
+      <c r="L76">
+        <v>224</v>
+      </c>
+      <c r="M76">
+        <v>157</v>
+      </c>
+      <c r="N76">
+        <v>203</v>
+      </c>
+      <c r="O76">
+        <v>54</v>
+      </c>
+      <c r="P76">
+        <v>134</v>
+      </c>
+      <c r="Q76">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A77" s="1">
+        <v>43974</v>
+      </c>
+      <c r="B77">
+        <v>1692</v>
+      </c>
+      <c r="C77">
+        <v>2367</v>
+      </c>
+      <c r="D77">
+        <v>190</v>
+      </c>
+      <c r="E77">
+        <v>154</v>
+      </c>
+      <c r="F77">
+        <v>41</v>
+      </c>
+      <c r="G77">
+        <v>240</v>
+      </c>
+      <c r="H77">
+        <v>458</v>
+      </c>
+      <c r="I77">
+        <v>20</v>
+      </c>
+      <c r="J77">
+        <v>571</v>
+      </c>
+      <c r="K77">
+        <v>1555</v>
+      </c>
+      <c r="L77">
+        <v>226</v>
+      </c>
+      <c r="M77">
+        <v>157</v>
+      </c>
+      <c r="N77">
+        <v>204</v>
+      </c>
+      <c r="O77">
+        <v>54</v>
+      </c>
+      <c r="P77">
+        <v>136</v>
+      </c>
+      <c r="Q77">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A78" s="1">
+        <v>43975</v>
+      </c>
+      <c r="B78">
+        <v>1697</v>
+      </c>
+      <c r="C78">
+        <v>2377</v>
+      </c>
+      <c r="D78">
+        <v>191</v>
+      </c>
+      <c r="E78">
+        <v>154</v>
+      </c>
+      <c r="F78">
+        <v>41</v>
+      </c>
+      <c r="G78">
+        <v>241</v>
+      </c>
+      <c r="H78">
+        <v>460</v>
+      </c>
+      <c r="I78">
+        <v>20</v>
+      </c>
+      <c r="J78">
+        <v>572</v>
+      </c>
+      <c r="K78">
+        <v>1563</v>
+      </c>
+      <c r="L78">
+        <v>227</v>
+      </c>
+      <c r="M78">
+        <v>157</v>
+      </c>
+      <c r="N78">
+        <v>204</v>
+      </c>
+      <c r="O78">
+        <v>54</v>
+      </c>
+      <c r="P78">
+        <v>137</v>
+      </c>
+      <c r="Q78">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A79" s="1">
+        <v>43976</v>
+      </c>
+      <c r="B79">
+        <v>1698</v>
+      </c>
+      <c r="C79">
+        <v>2382</v>
+      </c>
+      <c r="D79">
+        <v>191</v>
+      </c>
+      <c r="E79">
+        <v>154</v>
+      </c>
+      <c r="F79">
+        <v>41</v>
+      </c>
+      <c r="G79">
+        <v>241</v>
+      </c>
+      <c r="H79">
+        <v>460</v>
+      </c>
+      <c r="I79">
+        <v>20</v>
+      </c>
+      <c r="J79">
+        <v>572</v>
+      </c>
+      <c r="K79">
+        <v>1565</v>
+      </c>
+      <c r="L79">
+        <v>228</v>
+      </c>
+      <c r="M79">
+        <v>157</v>
+      </c>
+      <c r="N79">
+        <v>205</v>
+      </c>
+      <c r="O79">
+        <v>54</v>
+      </c>
+      <c r="P79">
+        <v>137</v>
+      </c>
+      <c r="Q79">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A80" s="1">
+        <v>43977</v>
+      </c>
+      <c r="B80">
+        <v>1707</v>
+      </c>
+      <c r="C80">
+        <v>2401</v>
+      </c>
+      <c r="D80">
+        <v>191</v>
+      </c>
+      <c r="E80">
+        <v>154</v>
+      </c>
+      <c r="F80">
+        <v>42</v>
+      </c>
+      <c r="G80">
+        <v>241</v>
+      </c>
+      <c r="H80">
+        <v>462</v>
+      </c>
+      <c r="I80">
+        <v>20</v>
+      </c>
+      <c r="J80">
+        <v>574</v>
+      </c>
+      <c r="K80">
+        <v>1571</v>
+      </c>
+      <c r="L80">
+        <v>228</v>
+      </c>
+      <c r="M80">
+        <v>158</v>
+      </c>
+      <c r="N80">
+        <v>207</v>
+      </c>
+      <c r="O80">
+        <v>54</v>
+      </c>
+      <c r="P80">
+        <v>139</v>
+      </c>
+      <c r="Q80">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A81" s="1">
+        <v>43978</v>
+      </c>
+      <c r="B81">
+        <v>1724</v>
+      </c>
+      <c r="C81">
+        <v>2404</v>
+      </c>
+      <c r="D81">
+        <v>193</v>
+      </c>
+      <c r="E81">
+        <v>154</v>
+      </c>
+      <c r="F81">
+        <v>42</v>
+      </c>
+      <c r="G81">
+        <v>242</v>
+      </c>
+      <c r="H81">
+        <v>466</v>
+      </c>
+      <c r="I81">
+        <v>20</v>
+      </c>
+      <c r="J81">
+        <v>578</v>
+      </c>
+      <c r="K81">
+        <v>1577</v>
+      </c>
+      <c r="L81">
+        <v>229</v>
+      </c>
+      <c r="M81">
+        <v>160</v>
+      </c>
+      <c r="N81">
+        <v>208</v>
+      </c>
+      <c r="O81">
+        <v>55</v>
+      </c>
+      <c r="P81">
+        <v>140</v>
+      </c>
+      <c r="Q81">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A82" s="1">
+        <v>43979</v>
+      </c>
+      <c r="B82">
+        <v>1724</v>
+      </c>
+      <c r="C82">
+        <v>2438</v>
+      </c>
+      <c r="D82">
+        <v>195</v>
+      </c>
+      <c r="E82">
+        <v>155</v>
+      </c>
+      <c r="F82">
+        <v>41</v>
+      </c>
+      <c r="G82">
+        <v>245</v>
+      </c>
+      <c r="H82">
+        <v>471</v>
+      </c>
+      <c r="I82">
+        <v>20</v>
+      </c>
+      <c r="J82">
+        <v>583</v>
+      </c>
+      <c r="K82">
+        <v>1582</v>
+      </c>
+      <c r="L82">
+        <v>230</v>
+      </c>
+      <c r="M82">
+        <v>161</v>
+      </c>
+      <c r="N82">
+        <v>210</v>
+      </c>
+      <c r="O82">
+        <v>55</v>
+      </c>
+      <c r="P82">
+        <v>143</v>
+      </c>
+      <c r="Q82">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A83" s="1">
+        <v>43980</v>
+      </c>
+      <c r="B83">
+        <v>1743</v>
+      </c>
+      <c r="C83">
+        <v>2441</v>
+      </c>
+      <c r="D83">
+        <v>196</v>
+      </c>
+      <c r="E83">
+        <v>155</v>
+      </c>
+      <c r="F83">
+        <v>41</v>
+      </c>
+      <c r="G83">
+        <v>246</v>
+      </c>
+      <c r="H83">
+        <v>476</v>
+      </c>
+      <c r="I83">
+        <v>20</v>
+      </c>
+      <c r="J83">
+        <v>585</v>
+      </c>
+      <c r="K83">
+        <v>1588</v>
+      </c>
+      <c r="L83">
+        <v>230</v>
+      </c>
+      <c r="M83">
+        <v>162</v>
+      </c>
+      <c r="N83">
+        <v>209</v>
+      </c>
+      <c r="O83">
+        <v>55</v>
+      </c>
+      <c r="P83">
+        <v>144</v>
+      </c>
+      <c r="Q83">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A84" s="1">
+        <v>43981</v>
+      </c>
+      <c r="B84">
+        <v>1748</v>
+      </c>
+      <c r="C84">
+        <v>2450</v>
+      </c>
+      <c r="D84">
+        <v>197</v>
+      </c>
+      <c r="E84">
+        <v>155</v>
+      </c>
+      <c r="F84">
+        <v>42</v>
+      </c>
+      <c r="G84">
+        <v>246</v>
+      </c>
+      <c r="H84">
+        <v>476</v>
+      </c>
+      <c r="I84">
+        <v>20</v>
+      </c>
+      <c r="J84">
+        <v>593</v>
+      </c>
+      <c r="K84">
+        <v>1595</v>
+      </c>
+      <c r="L84">
+        <v>230</v>
+      </c>
+      <c r="M84">
+        <v>163</v>
+      </c>
+      <c r="N84">
+        <v>213</v>
+      </c>
+      <c r="O84">
+        <v>55</v>
+      </c>
+      <c r="P84">
+        <v>145</v>
+      </c>
+      <c r="Q84">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A85" s="1">
+        <v>43982</v>
+      </c>
+      <c r="B85">
+        <v>1748</v>
+      </c>
+      <c r="C85">
+        <v>2450</v>
+      </c>
+      <c r="D85">
+        <v>198</v>
+      </c>
+      <c r="E85">
+        <v>155</v>
+      </c>
+      <c r="F85">
+        <v>42</v>
+      </c>
+      <c r="G85">
+        <v>252</v>
+      </c>
+      <c r="H85">
+        <v>477</v>
+      </c>
+      <c r="I85">
+        <v>20</v>
+      </c>
+      <c r="J85">
+        <v>593</v>
+      </c>
+      <c r="K85">
+        <v>1597</v>
+      </c>
+      <c r="L85">
+        <v>230</v>
+      </c>
+      <c r="M85">
+        <v>163</v>
+      </c>
+      <c r="N85">
+        <v>213</v>
+      </c>
+      <c r="O85">
+        <v>55</v>
+      </c>
+      <c r="P85">
+        <v>145</v>
+      </c>
+      <c r="Q85">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A86" s="1">
+        <v>43983</v>
+      </c>
+      <c r="B86">
+        <v>1752</v>
+      </c>
+      <c r="C86">
+        <v>2451</v>
+      </c>
+      <c r="D86">
+        <v>198</v>
+      </c>
+      <c r="E86">
+        <v>155</v>
+      </c>
+      <c r="F86">
+        <v>42</v>
+      </c>
+      <c r="G86">
+        <v>253</v>
+      </c>
+      <c r="H86">
+        <v>480</v>
+      </c>
+      <c r="I86">
+        <v>20</v>
+      </c>
+      <c r="J86">
+        <v>593</v>
+      </c>
+      <c r="K86">
+        <v>1598</v>
+      </c>
+      <c r="L86">
+        <v>230</v>
+      </c>
+      <c r="M86">
+        <v>163</v>
+      </c>
+      <c r="N86">
+        <v>214</v>
+      </c>
+      <c r="O86">
+        <v>55</v>
+      </c>
+      <c r="P86">
+        <v>145</v>
+      </c>
+      <c r="Q86">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A87" s="1">
+        <v>43984</v>
+      </c>
+      <c r="B87">
+        <v>1758</v>
+      </c>
+      <c r="C87">
+        <v>2456</v>
+      </c>
+      <c r="D87">
+        <v>198</v>
+      </c>
+      <c r="E87">
+        <v>155</v>
+      </c>
+      <c r="F87">
+        <v>42</v>
+      </c>
+      <c r="G87">
+        <v>253</v>
+      </c>
+      <c r="H87">
+        <v>480</v>
+      </c>
+      <c r="I87">
+        <v>20</v>
+      </c>
+      <c r="J87">
+        <v>594</v>
+      </c>
+      <c r="K87">
+        <v>1599</v>
+      </c>
+      <c r="L87">
+        <v>230</v>
+      </c>
+      <c r="M87">
+        <v>163</v>
+      </c>
+      <c r="N87">
+        <v>212</v>
+      </c>
+      <c r="O87">
+        <v>55</v>
+      </c>
+      <c r="P87">
+        <v>145</v>
+      </c>
+      <c r="Q87">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A88" s="1">
+        <v>43985</v>
+      </c>
+      <c r="B88">
+        <v>1760</v>
+      </c>
+      <c r="C88">
+        <v>2466</v>
+      </c>
+      <c r="D88">
+        <v>198</v>
+      </c>
+      <c r="E88">
+        <v>156</v>
+      </c>
+      <c r="F88">
+        <v>43</v>
+      </c>
+      <c r="G88">
+        <v>253</v>
+      </c>
+      <c r="H88">
+        <v>480</v>
+      </c>
+      <c r="I88">
+        <v>20</v>
+      </c>
+      <c r="J88">
+        <v>596</v>
+      </c>
+      <c r="K88">
+        <v>1607</v>
+      </c>
+      <c r="L88">
+        <v>230</v>
+      </c>
+      <c r="M88">
+        <v>163</v>
+      </c>
+      <c r="N88">
+        <v>212</v>
+      </c>
+      <c r="O88">
+        <v>55</v>
+      </c>
+      <c r="P88">
+        <v>146</v>
+      </c>
+      <c r="Q88">
+        <v>166</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>